<commit_message>
front - end modify
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meow\Desktop\LPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meow\Desktop\LPC\LPC_git\web_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B6C978-EB60-4106-A29F-DEBD419C1B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D95631-201A-4B70-8B0B-BE69CAE8D2DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="168" yWindow="1332" windowWidth="22320" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10464" yWindow="888" windowWidth="12528" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1206,7 @@
         <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>134</v>
@@ -1370,7 +1370,7 @@
         <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>99</v>

</xml_diff>